<commit_message>
Pruebas actualizadas y analizadas
</commit_message>
<xml_diff>
--- a/Documentation/Info Rendimiento Sprint 3.xlsx
+++ b/Documentation/Info Rendimiento Sprint 3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JdRod\Documents\Notifik\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Por Tareas" sheetId="1" r:id="rId1"/>
@@ -344,9 +344,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -356,6 +353,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,7 +439,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -509,7 +509,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-CO"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -542,41 +542,53 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Por Tareas'!$D$24:$D$27</c:f>
+              <c:f>'Por Tareas'!$D$23:$D$28</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>Inicio Sprint</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Entrega 1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Entrega 2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Entrega 3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Entrega 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fin Sprint</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Por Tareas'!$E$24:$E$27</c:f>
+              <c:f>'Por Tareas'!$E$23:$E$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -643,7 +655,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-CO"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -676,38 +688,53 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Por Tareas'!$D$24:$D$27</c:f>
+              <c:f>'Por Tareas'!$D$23:$D$28</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>Inicio Sprint</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Entrega 1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Entrega 2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Entrega 3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Entrega 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fin Sprint</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Por Tareas'!$F$24:$F$27</c:f>
+              <c:f>'Por Tareas'!$F$23:$F$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -725,11 +752,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="410716912"/>
-        <c:axId val="410715736"/>
+        <c:axId val="-111620944"/>
+        <c:axId val="-111632912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="410716912"/>
+        <c:axId val="-111620944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -769,10 +796,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="410715736"/>
+        <c:crossAx val="-111632912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -780,7 +807,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="410715736"/>
+        <c:axId val="-111632912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -816,7 +843,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="410716912"/>
+        <c:crossAx val="-111620944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -861,7 +888,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -907,7 +934,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -984,7 +1011,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1054,7 +1081,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-CO"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -1118,16 +1145,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -1200,7 +1227,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-CO"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -1264,7 +1291,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
@@ -1279,7 +1306,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1297,11 +1324,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="411155088"/>
-        <c:axId val="244327240"/>
+        <c:axId val="-111650320"/>
+        <c:axId val="-111622576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="411155088"/>
+        <c:axId val="-111650320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1341,10 +1368,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244327240"/>
+        <c:crossAx val="-111622576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1352,7 +1379,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244327240"/>
+        <c:axId val="-111622576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1388,7 +1415,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="411155088"/>
+        <c:crossAx val="-111650320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1433,7 +1460,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1479,7 +1506,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1561,7 +1588,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1713,11 +1740,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="246478336"/>
-        <c:axId val="246477944"/>
+        <c:axId val="-111649776"/>
+        <c:axId val="-111648688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246478336"/>
+        <c:axId val="-111649776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1757,10 +1784,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246477944"/>
+        <c:crossAx val="-111648688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1768,7 +1795,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246477944"/>
+        <c:axId val="-111648688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1816,10 +1843,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246478336"/>
+        <c:crossAx val="-111649776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1859,7 +1886,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1889,7 +1916,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4020,58 +4047,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.125" customWidth="1"/>
     <col min="8" max="8" width="3" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="35.42578125" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.875" customWidth="1"/>
+    <col min="10" max="10" width="35.375" customWidth="1"/>
+    <col min="11" max="11" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G3" s="11"/>
@@ -4108,12 +4135,12 @@
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
-      <c r="E5" s="25"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
-      <c r="J5" s="25"/>
+      <c r="J5" s="24"/>
       <c r="K5" s="14"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
@@ -4150,8 +4177,8 @@
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
@@ -4314,10 +4341,10 @@
       <c r="B22" s="14"/>
       <c r="C22" s="13"/>
       <c r="D22" s="16"/>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="21" t="s">
         <v>31</v>
       </c>
       <c r="G22" s="14"/>
@@ -4327,14 +4354,14 @@
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="13"/>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="24">
-        <v>7</v>
-      </c>
-      <c r="F23" s="24">
-        <v>7</v>
+      <c r="E23" s="23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="23">
+        <v>0</v>
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
@@ -4343,13 +4370,13 @@
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E24" s="19">
         <v>1</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="19">
         <v>2</v>
       </c>
       <c r="G24" s="14"/>
@@ -4359,13 +4386,13 @@
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="20">
-        <v>3</v>
-      </c>
-      <c r="F25" s="20">
+      <c r="E25" s="19">
+        <v>2</v>
+      </c>
+      <c r="F25" s="19">
         <v>5</v>
       </c>
       <c r="G25" s="14"/>
@@ -4375,13 +4402,13 @@
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="20">
-        <v>5</v>
-      </c>
-      <c r="F26" s="20">
+      <c r="E26" s="19">
+        <v>4</v>
+      </c>
+      <c r="F26" s="19">
         <v>5</v>
       </c>
       <c r="G26" s="14"/>
@@ -4391,13 +4418,15 @@
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="20">
+      <c r="E27" s="19">
+        <v>6</v>
+      </c>
+      <c r="F27" s="19">
         <v>7</v>
       </c>
-      <c r="F27" s="20"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
@@ -4405,13 +4434,13 @@
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="24">
-        <v>7</v>
-      </c>
-      <c r="F28" s="24">
+      <c r="E28" s="23">
+        <v>8</v>
+      </c>
+      <c r="F28" s="23">
         <v>7</v>
       </c>
       <c r="G28" s="14"/>
@@ -4429,10 +4458,10 @@
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
       <c r="D30" s="16"/>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="22" t="s">
+      <c r="F30" s="21" t="s">
         <v>30</v>
       </c>
       <c r="G30" s="14"/>
@@ -4442,14 +4471,14 @@
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="24">
-        <v>7</v>
-      </c>
-      <c r="F31" s="24">
-        <v>7</v>
+      <c r="E31" s="23">
+        <v>8</v>
+      </c>
+      <c r="F31" s="23">
+        <v>8</v>
       </c>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
@@ -4458,13 +4487,13 @@
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="20">
+      <c r="E32" s="19">
         <v>6</v>
       </c>
-      <c r="F32" s="20">
+      <c r="F32" s="19">
         <v>5</v>
       </c>
       <c r="G32" s="14"/>
@@ -4474,13 +4503,13 @@
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
-      <c r="D33" s="21" t="s">
+      <c r="D33" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="20">
-        <v>5</v>
-      </c>
-      <c r="F33" s="20">
+      <c r="E33" s="19">
+        <v>4</v>
+      </c>
+      <c r="F33" s="19">
         <v>2</v>
       </c>
       <c r="G33" s="14"/>
@@ -4488,36 +4517,36 @@
       <c r="I33" s="14"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="21" t="s">
+      <c r="D34" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="20">
-        <v>3</v>
-      </c>
-      <c r="F34" s="20">
+      <c r="E34" s="19">
         <v>2</v>
       </c>
+      <c r="F34" s="19">
+        <v>2</v>
+      </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E35" s="20">
+      <c r="E35" s="19">
         <v>1</v>
       </c>
-      <c r="F35" s="20">
+      <c r="F35" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="24">
+      <c r="E36" s="23">
         <v>0</v>
       </c>
-      <c r="F36" s="24">
-        <v>0</v>
+      <c r="F36" s="23">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4535,20 +4564,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -4559,7 +4588,7 @@
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="18" t="s">
         <v>21</v>
       </c>
       <c r="K4" s="12"/>

</xml_diff>